<commit_message>
Fixed Reg_No. Registration Number is now working properly
</commit_message>
<xml_diff>
--- a/Dummy_data4.xlsx
+++ b/Dummy_data4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\DBMS\DBMS Project\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6587FA27-6888-4084-BE6D-B6FBA0143FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83F7EB9-2D07-4672-A020-0EF1D74EE391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Registration No.</t>
   </si>
@@ -31,31 +31,106 @@
     <t>Date of Birth</t>
   </si>
   <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Father's Name</t>
+  </si>
+  <si>
+    <t>Previous School/ Instituion</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>Email Address</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Father's Name</t>
-  </si>
-  <si>
-    <t>Parent / Guardian Contact No.</t>
-  </si>
-  <si>
-    <t>Previous School/ Instituion</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>addd</t>
+  </si>
+  <si>
+    <t>papa</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>nsadnk</t>
+  </si>
+  <si>
+    <t>kjasds</t>
+  </si>
+  <si>
+    <t>naskdaskd</t>
+  </si>
+  <si>
+    <t>kakjdnasd</t>
+  </si>
+  <si>
+    <t>njksdsadb</t>
+  </si>
+  <si>
+    <t>hasdashd</t>
+  </si>
+  <si>
+    <t>badbabd</t>
+  </si>
+  <si>
+    <t>nkasdasad</t>
+  </si>
+  <si>
+    <t>name18</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>jasdnad</t>
+  </si>
+  <si>
+    <t>nasdnjad</t>
+  </si>
+  <si>
+    <t>jnakndajk</t>
+  </si>
+  <si>
+    <t>njaksndak</t>
+  </si>
+  <si>
+    <t>nasdkan</t>
+  </si>
+  <si>
+    <t>nasdnad</t>
+  </si>
+  <si>
+    <t>nasndand</t>
   </si>
 </sst>
 </file>
@@ -94,7 +169,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,28 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="1"/>
-    <col min="7" max="7" width="15.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="13.90625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +518,133 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed: Search bar is now working.
</commit_message>
<xml_diff>
--- a/Dummy_data4.xlsx
+++ b/Dummy_data4.xlsx
@@ -415,15 +415,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="1" min="1" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="1" min="2" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -838,6 +839,162 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>vytdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sfsfjg</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>fyaydfy</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>qu tstd</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>qauyu7</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>qgsdiuf7</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>gufs</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>hhagu</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>gasdgua</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>gahsdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>xzxzc</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ssf</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>avsdhv</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>whadh</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>vavdy</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>qvad</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>yqgdqv</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>vahgvdavd</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>adahgdv</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>jGSUY</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GAUD</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>UYF</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>UYQ</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>SU</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>GUWUYGD</t>
         </is>
       </c>
     </row>

</xml_diff>